<commit_message>
add new notional dataset
</commit_message>
<xml_diff>
--- a/day3/demo/datasets/Day 3 Data Dictionary.xlsx
+++ b/day3/demo/datasets/Day 3 Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stepheaneff/Documents/work/GT/data-science-basics-2023/day3/demo/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BA135D-F226-2A41-A662-5DD86137C7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D928016-8EB1-3745-A1BD-D5DC41CC410E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="760" windowWidth="29780" windowHeight="16820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="760" windowWidth="29780" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table information" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="267">
   <si>
     <t>Text</t>
   </si>
@@ -489,9 +489,6 @@
     <t>This data dictionary is intended to document the dataset(s) accessible at https://github.com/seaneff/data-science-basics-2023/tree/main/day3/demo/datasets</t>
   </si>
   <si>
-    <t>The data dictionary was last updated on June 14, 2023</t>
-  </si>
-  <si>
     <t>countries</t>
   </si>
   <si>
@@ -772,13 +769,82 @@
   </si>
   <si>
     <t>Steph Eaneff</t>
+  </si>
+  <si>
+    <t>Added information on notional (fake) study data</t>
+  </si>
+  <si>
+    <t>Needed to generate notional (fake) study data for new plot types</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>A fake ("notional") dataset with summary information on an imaginary study</t>
+  </si>
+  <si>
+    <t>one row per group per week</t>
+  </si>
+  <si>
+    <t>Developed for use as a teaching tool, data are entirely fake</t>
+  </si>
+  <si>
+    <t>The data dictionary was last updated on August 16, 2023</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>average_score</t>
+  </si>
+  <si>
+    <t>ci_lower</t>
+  </si>
+  <si>
+    <t>ci_upper</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Average score</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Lower confidence interval (95%)</t>
+  </si>
+  <si>
+    <t>Upper confidence interval (95%)</t>
+  </si>
+  <si>
+    <t>The time of the observation</t>
+  </si>
+  <si>
+    <t>The group for which the average score was calculated</t>
+  </si>
+  <si>
+    <t>The average score of the group</t>
+  </si>
+  <si>
+    <t>The lower bound of a 95% confidence interval for the average score</t>
+  </si>
+  <si>
+    <t>The upper bound of a 95% confidence interval for the average score</t>
+  </si>
+  <si>
+    <t>Data are fake ("notional")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -868,12 +934,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri (Body)"/>
@@ -882,6 +942,30 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -947,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -984,31 +1068,22 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1025,6 +1100,21 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1303,8 +1393,8 @@
   </sheetPr>
   <dimension ref="A1:V1002"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1317,26 +1407,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="124" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25"/>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
     </row>
     <row r="3" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
+      <c r="A3" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
     </row>
     <row r="4" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
@@ -1345,17 +1435,17 @@
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:22" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
     </row>
     <row r="6" spans="1:22" ht="32.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>2</v>
@@ -1372,19 +1462,19 @@
     </row>
     <row r="7" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>152</v>
-      </c>
       <c r="E7" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1406,19 +1496,19 @@
     </row>
     <row r="8" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>159</v>
-      </c>
       <c r="D8" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1440,19 +1530,19 @@
     </row>
     <row r="9" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="D9" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1473,11 +1563,21 @@
       <c r="V9" s="2"/>
     </row>
     <row r="10" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>249</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -3544,1633 +3644,1703 @@
   </sheetPr>
   <dimension ref="A1:V998"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.796875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="55.796875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="40.19921875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="59.796875" style="16" customWidth="1"/>
-    <col min="5" max="5" width="30" style="16" customWidth="1"/>
-    <col min="6" max="6" width="27.796875" style="16" customWidth="1"/>
-    <col min="7" max="7" width="45.19921875" style="16" customWidth="1"/>
-    <col min="8" max="16384" width="14.3984375" style="16"/>
+    <col min="1" max="1" width="25.796875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="55.796875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="40.19921875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="59.796875" style="15" customWidth="1"/>
+    <col min="5" max="5" width="30" style="15" customWidth="1"/>
+    <col min="6" max="6" width="27.796875" style="15" customWidth="1"/>
+    <col min="7" max="7" width="45.19921875" style="15" customWidth="1"/>
+    <col min="8" max="16384" width="14.3984375" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:22" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-    </row>
-    <row r="3" spans="1:22" s="22" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+    </row>
+    <row r="3" spans="1:22" s="19" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="18" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+    </row>
+    <row r="5" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C5" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+    </row>
+    <row r="6" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+    </row>
+    <row r="7" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+    </row>
+    <row r="8" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+    </row>
+    <row r="9" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+    </row>
+    <row r="10" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+    </row>
+    <row r="11" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+    </row>
+    <row r="12" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+    </row>
+    <row r="13" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+    </row>
+    <row r="14" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+    </row>
+    <row r="15" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+    </row>
+    <row r="16" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+    </row>
+    <row r="17" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+    </row>
+    <row r="18" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+    </row>
+    <row r="19" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
+    </row>
+    <row r="20" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+    </row>
+    <row r="21" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="D21" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E21" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="F21" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="G21" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
+    </row>
+    <row r="22" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="D22" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+    </row>
+    <row r="23" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-    </row>
-    <row r="5" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B5" s="15" t="s">
+      <c r="B23" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="E5" s="18" t="s">
+      <c r="C23" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F23" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G5" s="18" t="s">
+      <c r="G23" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+    </row>
+    <row r="24" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+    </row>
+    <row r="25" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+    </row>
+    <row r="26" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+    </row>
+    <row r="27" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="E27" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-    </row>
-    <row r="6" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="F27" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="G27" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="16"/>
+      <c r="V27" s="16"/>
+    </row>
+    <row r="28" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F28" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-    </row>
-    <row r="7" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="C7" s="17" t="s">
+      <c r="G28" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="16"/>
+    </row>
+    <row r="29" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+      <c r="U29" s="16"/>
+      <c r="V29" s="16"/>
+    </row>
+    <row r="30" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="16"/>
+      <c r="U30" s="16"/>
+      <c r="V30" s="16"/>
+    </row>
+    <row r="31" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16"/>
+      <c r="V31" s="16"/>
+    </row>
+    <row r="32" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="16"/>
+      <c r="T32" s="16"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="16"/>
+    </row>
+    <row r="33" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F33" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G33" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+    </row>
+    <row r="34" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G34" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
+      <c r="V34" s="16"/>
+    </row>
+    <row r="35" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="G35" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
+    </row>
+    <row r="36" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="E36" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="F36" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16"/>
+      <c r="V36" s="16"/>
+    </row>
+    <row r="37" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="E37" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="F37" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-    </row>
-    <row r="8" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="E8" s="18" t="s">
+      <c r="G37" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+      <c r="T37" s="16"/>
+      <c r="U37" s="16"/>
+      <c r="V37" s="16"/>
+    </row>
+    <row r="38" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="E38" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F38" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-    </row>
-    <row r="9" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-    </row>
-    <row r="10" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-    </row>
-    <row r="11" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-    </row>
-    <row r="12" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-    </row>
-    <row r="13" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-    </row>
-    <row r="14" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-    </row>
-    <row r="15" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>216</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-    </row>
-    <row r="16" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-    </row>
-    <row r="17" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-    </row>
-    <row r="18" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-    </row>
-    <row r="19" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-    </row>
-    <row r="20" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
-      <c r="U20" s="18"/>
-      <c r="V20" s="18"/>
-    </row>
-    <row r="21" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="18"/>
-      <c r="V21" s="18"/>
-    </row>
-    <row r="22" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-    </row>
-    <row r="23" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
-      <c r="T23" s="18"/>
-      <c r="U23" s="18"/>
-      <c r="V23" s="18"/>
-    </row>
-    <row r="24" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
-      <c r="T24" s="18"/>
-      <c r="U24" s="18"/>
-      <c r="V24" s="18"/>
-    </row>
-    <row r="25" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="18"/>
-      <c r="T25" s="18"/>
-      <c r="U25" s="18"/>
-      <c r="V25" s="18"/>
-    </row>
-    <row r="26" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="18"/>
-      <c r="U26" s="18"/>
-      <c r="V26" s="18"/>
-    </row>
-    <row r="27" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="18"/>
-      <c r="U27" s="18"/>
-      <c r="V27" s="18"/>
-    </row>
-    <row r="28" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G28" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
-      <c r="T28" s="18"/>
-      <c r="U28" s="18"/>
-      <c r="V28" s="18"/>
-    </row>
-    <row r="29" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="18"/>
-      <c r="T29" s="18"/>
-      <c r="U29" s="18"/>
-      <c r="V29" s="18"/>
-    </row>
-    <row r="30" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F30" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
-      <c r="U30" s="18"/>
-      <c r="V30" s="18"/>
-    </row>
-    <row r="31" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="18"/>
-      <c r="U31" s="18"/>
-      <c r="V31" s="18"/>
-    </row>
-    <row r="32" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-    </row>
-    <row r="33" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
-      <c r="U33" s="18"/>
-      <c r="V33" s="18"/>
-    </row>
-    <row r="34" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
-      <c r="T34" s="18"/>
-      <c r="U34" s="18"/>
-      <c r="V34" s="18"/>
-    </row>
-    <row r="35" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
-      <c r="T35" s="18"/>
-      <c r="U35" s="18"/>
-      <c r="V35" s="18"/>
-    </row>
-    <row r="36" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
-      <c r="T36" s="18"/>
-      <c r="U36" s="18"/>
-      <c r="V36" s="18"/>
-    </row>
-    <row r="37" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
-      <c r="T37" s="18"/>
-      <c r="U37" s="18"/>
-      <c r="V37" s="18"/>
-    </row>
-    <row r="38" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="18"/>
-      <c r="U38" s="18"/>
-      <c r="V38" s="18"/>
+      <c r="G38" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
+      <c r="V38" s="16"/>
     </row>
     <row r="39" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
-      <c r="V39" s="18"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
+      <c r="V39" s="16"/>
     </row>
     <row r="40" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="U40" s="18"/>
-      <c r="V40" s="18"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
+      <c r="Q40" s="16"/>
+      <c r="R40" s="16"/>
+      <c r="S40" s="16"/>
+      <c r="T40" s="16"/>
+      <c r="U40" s="16"/>
+      <c r="V40" s="16"/>
     </row>
     <row r="41" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="18"/>
-      <c r="U41" s="18"/>
-      <c r="V41" s="18"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="16"/>
+      <c r="T41" s="16"/>
+      <c r="U41" s="16"/>
+      <c r="V41" s="16"/>
     </row>
     <row r="42" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
-      <c r="U42" s="18"/>
-      <c r="V42" s="18"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="16"/>
+      <c r="V42" s="16"/>
     </row>
     <row r="43" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="18"/>
-      <c r="U43" s="18"/>
-      <c r="V43" s="18"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="16"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="16"/>
     </row>
     <row r="44" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="18"/>
-      <c r="U44" s="18"/>
-      <c r="V44" s="18"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+      <c r="Q44" s="16"/>
+      <c r="R44" s="16"/>
+      <c r="S44" s="16"/>
+      <c r="T44" s="16"/>
+      <c r="U44" s="16"/>
+      <c r="V44" s="16"/>
     </row>
     <row r="45" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-      <c r="T45" s="18"/>
-      <c r="U45" s="18"/>
-      <c r="V45" s="18"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="16"/>
+      <c r="R45" s="16"/>
+      <c r="S45" s="16"/>
+      <c r="T45" s="16"/>
+      <c r="U45" s="16"/>
+      <c r="V45" s="16"/>
     </row>
     <row r="46" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-      <c r="T46" s="18"/>
-      <c r="U46" s="18"/>
-      <c r="V46" s="18"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+      <c r="T46" s="16"/>
+      <c r="U46" s="16"/>
+      <c r="V46" s="16"/>
     </row>
     <row r="47" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="18"/>
-      <c r="U47" s="18"/>
-      <c r="V47" s="18"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16"/>
+      <c r="R47" s="16"/>
+      <c r="S47" s="16"/>
+      <c r="T47" s="16"/>
+      <c r="U47" s="16"/>
+      <c r="V47" s="16"/>
     </row>
     <row r="48" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="18"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
-      <c r="M48" s="18"/>
-      <c r="N48" s="18"/>
-      <c r="O48" s="18"/>
-      <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
-      <c r="T48" s="18"/>
-      <c r="U48" s="18"/>
-      <c r="V48" s="18"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="16"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+      <c r="Q48" s="16"/>
+      <c r="R48" s="16"/>
+      <c r="S48" s="16"/>
+      <c r="T48" s="16"/>
+      <c r="U48" s="16"/>
+      <c r="V48" s="16"/>
     </row>
     <row r="49" spans="1:22" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="18"/>
-      <c r="M49" s="18"/>
-      <c r="N49" s="18"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="18"/>
-      <c r="Q49" s="18"/>
-      <c r="R49" s="18"/>
-      <c r="S49" s="18"/>
-      <c r="T49" s="18"/>
-      <c r="U49" s="18"/>
-      <c r="V49" s="18"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="16"/>
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+      <c r="Q49" s="16"/>
+      <c r="R49" s="16"/>
+      <c r="S49" s="16"/>
+      <c r="T49" s="16"/>
+      <c r="U49" s="16"/>
+      <c r="V49" s="16"/>
     </row>
     <row r="50" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
-      <c r="N50" s="18"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="18"/>
-      <c r="Q50" s="18"/>
-      <c r="R50" s="18"/>
-      <c r="S50" s="18"/>
-      <c r="T50" s="18"/>
-      <c r="U50" s="18"/>
-      <c r="V50" s="18"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
+      <c r="L50" s="16"/>
+      <c r="M50" s="16"/>
+      <c r="N50" s="16"/>
+      <c r="O50" s="16"/>
+      <c r="P50" s="16"/>
+      <c r="Q50" s="16"/>
+      <c r="R50" s="16"/>
+      <c r="S50" s="16"/>
+      <c r="T50" s="16"/>
+      <c r="U50" s="16"/>
+      <c r="V50" s="16"/>
     </row>
     <row r="51" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="18"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="18"/>
-      <c r="M51" s="18"/>
-      <c r="N51" s="18"/>
-      <c r="O51" s="18"/>
-      <c r="P51" s="18"/>
-      <c r="Q51" s="18"/>
-      <c r="R51" s="18"/>
-      <c r="S51" s="18"/>
-      <c r="T51" s="18"/>
-      <c r="U51" s="18"/>
-      <c r="V51" s="18"/>
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
+      <c r="L51" s="16"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="16"/>
+      <c r="P51" s="16"/>
+      <c r="Q51" s="16"/>
+      <c r="R51" s="16"/>
+      <c r="S51" s="16"/>
+      <c r="T51" s="16"/>
+      <c r="U51" s="16"/>
+      <c r="V51" s="16"/>
     </row>
     <row r="52" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="53" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6154,13 +6324,13 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:19" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:19" ht="38" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -8173,7 +8343,7 @@
   <dimension ref="A1:S999"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8190,13 +8360,13 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:19" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:19" ht="38" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -8216,17 +8386,17 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23">
+      <c r="A4" s="20">
         <v>45091</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="25" t="s">
         <v>243</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>244</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -8245,10 +8415,18 @@
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:19" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="20">
+        <v>45154</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>243</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>

</xml_diff>